<commit_message>
KYC details pages added
</commit_message>
<xml_diff>
--- a/mymoneykart/src/test/resources/SiteTestData.xlsx
+++ b/mymoneykart/src/test/resources/SiteTestData.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="74">
   <si>
     <t>User Name</t>
   </si>
@@ -32,10 +32,7 @@
     <t>123456</t>
   </si>
   <si>
-    <t>arjun@gmail.com</t>
-  </si>
-  <si>
-    <t>Arjun@123</t>
+    <t>9741638520</t>
   </si>
   <si>
     <t>narendra.h.rajput@trimantrallp.com</t>
@@ -384,7 +381,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -410,28 +407,26 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="arjun@gmail.com"/>
-    <hyperlink ref="B3" r:id="rId2" display="Arjun@123"/>
-    <hyperlink ref="A4" r:id="rId3" display="narendra.h.rajput@trimantrallp.com"/>
-    <hyperlink ref="B4" r:id="rId4" display="Narendra@123"/>
+    <hyperlink ref="A4" r:id="rId1" display="narendra.h.rajput@trimantrallp.com"/>
+    <hyperlink ref="B4" r:id="rId2" display="Narendra@123"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -451,7 +446,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="B3 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -464,35 +459,35 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="C3" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -514,7 +509,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="G11" activeCellId="1" sqref="B3 G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -530,107 +525,107 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -658,7 +653,7 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K18" activeCellId="0" sqref="K18"/>
+      <selection pane="topLeft" activeCell="K18" activeCellId="1" sqref="B3 K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -676,152 +671,152 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O2" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="M2" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="O2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="G3" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="N3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="M3" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>74</v>
-      </c>
       <c r="P3" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bus Home page functionality added
</commit_message>
<xml_diff>
--- a/mymoneykart/src/test/resources/SiteTestData.xlsx
+++ b/mymoneykart/src/test/resources/SiteTestData.xlsx
@@ -446,7 +446,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="B3 C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -509,7 +509,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="1" sqref="B3 G11"/>
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -653,7 +653,7 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K18" activeCellId="1" sqref="B3 K18"/>
+      <selection pane="topLeft" activeCell="K18" activeCellId="0" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>